<commit_message>
avancé modeste, envoie de l'appli a christophe,début du RGPD (ca devrait pas être long)
</commit_message>
<xml_diff>
--- a/Conception/PlanDeTest.xlsx
+++ b/Conception/PlanDeTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2cfcaab5c8ed795/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{06151501-CBDD-4D07-96A8-B2899AD16C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF3B5151-F7DA-4913-99BA-EF50EB9ADEDB}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{06151501-CBDD-4D07-96A8-B2899AD16C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{003CE63D-25AA-4AC0-83DA-C191F81FD5BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27EA1B9A-3EFA-48B8-8711-25AA78E37CA3}"/>
+    <workbookView xWindow="2205" yWindow="2295" windowWidth="26595" windowHeight="11295" xr2:uid="{27EA1B9A-3EFA-48B8-8711-25AA78E37CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="71">
   <si>
     <t>Fonctionnalité majeure</t>
   </si>
@@ -183,6 +183,72 @@
   </si>
   <si>
     <t>Paramétrage de l'envoie de mail</t>
+  </si>
+  <si>
+    <t>Paramétrage de l'accés au mail</t>
+  </si>
+  <si>
+    <t>Création d'un paramétrage</t>
+  </si>
+  <si>
+    <t>Mise a jour d'un paramétrage</t>
+  </si>
+  <si>
+    <t>Unicité du paramétrage pour un magasin</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Limitation de l'accés au Admin</t>
+  </si>
+  <si>
+    <t>Limitation de l'accés a la creation de magasin aux superadmins</t>
+  </si>
+  <si>
+    <t>Gestion des clients</t>
+  </si>
+  <si>
+    <t>Supprimer un client</t>
+  </si>
+  <si>
+    <t>Mettre à jour un client</t>
+  </si>
+  <si>
+    <t>Créer un utilisateur</t>
+  </si>
+  <si>
+    <t>Créer un magasin</t>
+  </si>
+  <si>
+    <t>Supprimer un utilisateur (superadmin uniquement)</t>
+  </si>
+  <si>
+    <t>Supprimer un magasin( superadmin uniquement)</t>
+  </si>
+  <si>
+    <t>Gestion du visuel</t>
+  </si>
+  <si>
+    <t>Paramétrage de la couleur du background</t>
+  </si>
+  <si>
+    <t>Paramétrage de la couleur du menu</t>
+  </si>
+  <si>
+    <t>Paramétrage de la couleur du text</t>
+  </si>
+  <si>
+    <t>Tableau récapitulatif</t>
+  </si>
+  <si>
+    <t>Génerer un tableau récapitulatif des ventes</t>
+  </si>
+  <si>
+    <t>Filtrer par évennement</t>
   </si>
 </sst>
 </file>
@@ -224,12 +290,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -253,6 +322,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD7F829-C36B-44AE-B322-D33CDEB3579A}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +654,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -590,36 +663,48 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D3" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -628,18 +713,24 @@
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D7" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -648,27 +739,36 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D9" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D10" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -677,54 +777,72 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D12" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D13" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D14" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D15" s="3">
+        <v>45138</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="D16" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -733,27 +851,36 @@
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="D17" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="D18" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="D19" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -762,54 +889,72 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="D20" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="D21" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="D22" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="D23" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="D24" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="D25" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -818,27 +963,36 @@
       <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="D26" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="D27" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="D28" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -847,65 +1001,342 @@
       <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="D29" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45140</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A48"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>

</xml_diff>